<commit_message>
resolved testData issue and added Seperate sheet for each module
</commit_message>
<xml_diff>
--- a/com.ElfBatch14/src/test/resources/testdata.xlsx
+++ b/com.ElfBatch14/src/test/resources/testdata.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumanth\git\ElfBatch-14\com.ElfBatch14\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4185" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14360" windowHeight="4190" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Contacts" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Contacts" sheetId="2" r:id="rId1"/>
+    <sheet name="Invoice" sheetId="1" r:id="rId2"/>
+    <sheet name="Leads" sheetId="3" r:id="rId3"/>
+    <sheet name="Organisation" sheetId="4" r:id="rId4"/>
+    <sheet name="Products" sheetId="5" r:id="rId5"/>
+    <sheet name="PurchaseOder" sheetId="6" r:id="rId6"/>
+    <sheet name="SalesOrder" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>devika</t>
   </si>
@@ -29,15 +38,77 @@
   <si>
     <t>Bagoji</t>
   </si>
+  <si>
+    <t>Mr.</t>
+  </si>
+  <si>
+    <t>vishwa</t>
+  </si>
+  <si>
+    <t>bagoji</t>
+  </si>
+  <si>
+    <t>idrive</t>
+  </si>
+  <si>
+    <t>dev</t>
+  </si>
+  <si>
+    <t>bnvfvxdfvc@gmail.com</t>
+  </si>
+  <si>
+    <t>nbbb@gmail.com</t>
+  </si>
+  <si>
+    <t>www.abc.com</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>abcdef</t>
+  </si>
+  <si>
+    <t>ghijka</t>
+  </si>
+  <si>
+    <t>jkhkjhjkh</t>
+  </si>
+  <si>
+    <t>iuhyugj</t>
+  </si>
+  <si>
+    <t>mnjbghcfgxdfzdszszsd</t>
+  </si>
+  <si>
+    <t>rakshit</t>
+  </si>
+  <si>
+    <t>rashid</t>
+  </si>
+  <si>
+    <t>google</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -60,13 +131,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -74,6 +157,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -122,7 +208,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -157,7 +243,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -366,29 +452,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -396,7 +468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -404,7 +476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -417,13 +489,163 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A6:T8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1">
+        <v>9999</v>
+      </c>
+      <c r="G6" s="1">
+        <v>9</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="3">
+        <v>99999999</v>
+      </c>
+      <c r="J6" s="4">
+        <v>9090897897</v>
+      </c>
+      <c r="K6" s="3">
+        <v>8888</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6">
+        <v>777</v>
+      </c>
+      <c r="P6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>14</v>
+      </c>
+      <c r="R6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S6" t="s">
+        <v>16</v>
+      </c>
+      <c r="T6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H6" r:id="rId1"/>
+    <hyperlink ref="L6" r:id="rId2"/>
+    <hyperlink ref="M6" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding Leads module testscript and repository and updated excel util.
</commit_message>
<xml_diff>
--- a/com.ElfBatch14/src/test/resources/testdata.xlsx
+++ b/com.ElfBatch14/src/test/resources/testdata.xlsx
@@ -1,15 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumanth\git\ElfBatch-14\com.ElfBatch14\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0D3A5467-1E41-4A65-B438-6420218F856C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14360" windowHeight="4190" activeTab="2"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="14388" windowHeight="7536" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="2" r:id="rId1"/>
@@ -20,7 +16,8 @@
     <sheet name="PurchaseOder" sheetId="6" r:id="rId6"/>
     <sheet name="SalesOrder" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:Q24"/>
 </workbook>
 </file>
 
@@ -93,7 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -241,6 +238,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -276,6 +290,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -451,16 +482,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -468,7 +499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -476,7 +507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -490,30 +521,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A6:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -575,12 +606,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -593,59 +624,59 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1"/>
-    <hyperlink ref="L6" r:id="rId2"/>
-    <hyperlink ref="M6" r:id="rId3"/>
+    <hyperlink ref="H6" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="L6" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="M6" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added test data, updated test Script and created object for selectutil in basetest
</commit_message>
<xml_diff>
--- a/com.ElfBatch14/src/test/resources/testdata.xlsx
+++ b/com.ElfBatch14/src/test/resources/testdata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0D3A5467-1E41-4A65-B438-6420218F856C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{EAC349A0-ABC3-4509-A6AF-E0921AF48DE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="14388" windowHeight="7536" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="6015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="2" r:id="rId1"/>
@@ -17,12 +17,12 @@
     <sheet name="SalesOrder" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:Q24"/>
+  <oleSize ref="A1:Q18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>devika</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>google</t>
+  </si>
+  <si>
+    <t>aaj singh</t>
+  </si>
+  <si>
+    <t>raj singh</t>
+  </si>
+  <si>
+    <t>akash</t>
+  </si>
+  <si>
+    <t>piyush</t>
   </si>
 </sst>
 </file>
@@ -483,15 +495,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B4"/>
+  <dimension ref="A2:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -499,7 +511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -507,12 +519,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -528,7 +565,7 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -538,13 +575,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A6:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -606,12 +643,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -638,7 +675,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -650,7 +687,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -662,7 +699,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -676,7 +713,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TestScripts,PropertyFileUtil ,ProductPage and testdata is added
</commit_message>
<xml_diff>
--- a/com.ElfBatch14/src/test/resources/testdata.xlsx
+++ b/com.ElfBatch14/src/test/resources/testdata.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0D3A5467-1E41-4A65-B438-6420218F856C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="14388" windowHeight="7536" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="17250" windowHeight="5850" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="2" r:id="rId1"/>
@@ -16,13 +15,19 @@
     <sheet name="PurchaseOder" sheetId="6" r:id="rId6"/>
     <sheet name="SalesOrder" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
   <oleSize ref="A1:Q24"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+  <si>
+    <t>shraddha</t>
+  </si>
+  <si>
+    <t>Bagoji</t>
+  </si>
   <si>
     <t>devika</t>
   </si>
@@ -30,12 +35,6 @@
     <t>patel</t>
   </si>
   <si>
-    <t>shraddha</t>
-  </si>
-  <si>
-    <t>Bagoji</t>
-  </si>
-  <si>
     <t>Mr.</t>
   </si>
   <si>
@@ -85,21 +84,50 @@
   </si>
   <si>
     <t>google</t>
+  </si>
+  <si>
+    <t>Pendriver</t>
+  </si>
+  <si>
+    <t>Pd-001</t>
+  </si>
+  <si>
+    <t>deit/del</t>
+  </si>
+  <si>
+    <t>Pd-002</t>
+  </si>
+  <si>
+    <t>Pd-003</t>
+  </si>
+  <si>
+    <t>pd-004</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -107,19 +135,341 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -127,36 +477,319 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -205,7 +838,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -238,26 +871,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,23 +906,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -477,74 +1076,78 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A6:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7"/>
   <sheetData>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -560,28 +1163,28 @@
       <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <v>9999</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>9</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="4">
         <v>99999999</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="5">
         <v>9090897897</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="4">
         <v>8888</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="N6" t="s">
@@ -606,12 +1209,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -624,60 +1227,177 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="L6" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="M6" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="H6" r:id="rId1" display="bnvfvxdfvc@gmail.com"/>
+    <hyperlink ref="L6" r:id="rId2" display="nbbb@gmail.com"/>
+    <hyperlink ref="M6" r:id="rId3" display="www.abc.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A6:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:G10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetData>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1">
+        <v>232</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>343</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1">
+        <v>233</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>234</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1">
+        <v>234</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>134</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1">
+        <v>235</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>354</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>